<commit_message>
ENH: download image using axios and page screenshot
</commit_message>
<xml_diff>
--- a/dailyCoding/nodejs-crawler/xlsx/result.xlsx
+++ b/dailyCoding/nodejs-crawler/xlsx/result.xlsx
@@ -398,9 +398,6 @@
       <c r="B2" t="str">
         <v>https://movie.naver.com/movie/bi/mi/basic.nhn?code=72363</v>
       </c>
-      <c r="C2">
-        <v>8.8</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -409,9 +406,6 @@
       <c r="B3" t="str">
         <v>https://movie.naver.com/movie/bi/mi/basic.nhn?code=100931</v>
       </c>
-      <c r="C3">
-        <v>9.12</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -420,9 +414,6 @@
       <c r="B4" t="str">
         <v>https://movie.naver.com/movie/bi/mi/basic.nhn?code=61521</v>
       </c>
-      <c r="C4">
-        <v>8.85</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -431,9 +422,6 @@
       <c r="B5" t="str">
         <v>https://movie.naver.com/movie/bi/mi/basic.nhn?code=30688</v>
       </c>
-      <c r="C5">
-        <v>9.25</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -441,9 +429,6 @@
       </c>
       <c r="B6" t="str">
         <v>https://movie.naver.com/movie/bi/mi/basic.nhn?code=37148</v>
-      </c>
-      <c r="C6">
-        <v>9.07</v>
       </c>
     </row>
   </sheetData>

</xml_diff>